<commit_message>
Screen changes - hot deals annd ad banner
</commit_message>
<xml_diff>
--- a/src/assets/ItemDetails.xlsx
+++ b/src/assets/ItemDetails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SunnSid/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4E33F6-32A4-284F-A191-361C86C16DED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B70EDC-EA43-8840-B9CA-5B336456C4D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15960" xr2:uid="{014425C1-AE4C-E642-9F77-EDAE2C3E7B19}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Item Name</t>
   </si>
@@ -36,51 +37,80 @@
     <t>Item Price</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Sona Masuri</t>
-  </si>
-  <si>
-    <t>Dal</t>
-  </si>
-  <si>
-    <t>Chana</t>
-  </si>
-  <si>
-    <t>Roti</t>
-  </si>
-  <si>
-    <t>Wheat</t>
+    <t>Item Id</t>
+  </si>
+  <si>
+    <t>Item weight</t>
+  </si>
+  <si>
+    <t>Item quantity</t>
+  </si>
+  <si>
+    <t>Product Category</t>
+  </si>
+  <si>
+    <t>Discount Price</t>
+  </si>
+  <si>
+    <t>noodles</t>
+  </si>
+  <si>
+    <t>indiagaterice</t>
+  </si>
+  <si>
+    <t>mangoes</t>
   </si>
   <si>
     <t>Maggi</t>
   </si>
   <si>
-    <t>Item Id</t>
-  </si>
-  <si>
-    <t>I like Maggi</t>
-  </si>
-  <si>
-    <t>Item weight</t>
-  </si>
-  <si>
-    <t>Item quantity</t>
-  </si>
-  <si>
-    <t>Product Category</t>
-  </si>
-  <si>
-    <t>Discount Price</t>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>Rusks</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>eggplant</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>soup</t>
+  </si>
+  <si>
+    <t>strawberry</t>
+  </si>
+  <si>
+    <t>sweetcorn</t>
+  </si>
+  <si>
+    <t>cookies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,8 +138,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,145 +455,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E319F24-2E3F-2840-A207-856C21D01818}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>20.9</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>10.7</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>30.8</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>17</v>
+      <c r="H15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fetch image by image name
</commit_message>
<xml_diff>
--- a/src/assets/ItemDetails.xlsx
+++ b/src/assets/ItemDetails.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SunnSid/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B70EDC-EA43-8840-B9CA-5B336456C4D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3028E313-91EB-5F40-941C-C902C0F3E53C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15960" xr2:uid="{014425C1-AE4C-E642-9F77-EDAE2C3E7B19}"/>
+    <workbookView xWindow="1120" yWindow="6660" windowWidth="28040" windowHeight="15960" xr2:uid="{014425C1-AE4C-E642-9F77-EDAE2C3E7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
   <si>
     <t>Item Name</t>
   </si>
@@ -95,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Image Name</t>
+  </si>
+  <si>
+    <t>Dal</t>
   </si>
 </sst>
 </file>
@@ -455,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E319F24-2E3F-2840-A207-856C21D01818}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +478,7 @@
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -498,8 +503,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -519,10 +527,13 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -544,8 +555,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -565,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -591,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>12</v>
@@ -615,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -638,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -661,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -684,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -707,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -730,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -753,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -773,10 +787,10 @@
         <v>2</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -799,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -819,6 +833,972 @@
         <v>3</v>
       </c>
       <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>500</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>500</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46">
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48">
+        <v>9</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>500</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55">
+        <v>9</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Images Save and update in tables
</commit_message>
<xml_diff>
--- a/src/assets/ItemDetails.xlsx
+++ b/src/assets/ItemDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SunnSid/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3028E313-91EB-5F40-941C-C902C0F3E53C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E527745-207E-D14D-B8DC-360D30C06501}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="6660" windowWidth="28040" windowHeight="15960" xr2:uid="{014425C1-AE4C-E642-9F77-EDAE2C3E7B19}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{014425C1-AE4C-E642-9F77-EDAE2C3E7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="24">
   <si>
     <t>Item Name</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Image Name</t>
-  </si>
-  <si>
-    <t>Dal</t>
   </si>
 </sst>
 </file>
@@ -463,7 +460,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,6 +473,7 @@
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -529,8 +527,9 @@
       <c r="H2">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
+      <c r="I2" t="str">
+        <f>CONCATENATE(B2,".png")</f>
+        <v>Maggi.png</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -555,8 +554,9 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
+      <c r="I3" t="str">
+        <f>CONCATENATE(B3,".png")</f>
+        <v>noodles.png</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -581,6 +581,10 @@
       <c r="H4">
         <v>5</v>
       </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I57" si="0">CONCATENATE(B4,".png")</f>
+        <v>indiagaterice.png</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -603,6 +607,10 @@
       </c>
       <c r="H5">
         <v>0</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>mangoes.png</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -628,6 +636,10 @@
       <c r="H6">
         <v>0</v>
       </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>onion.png</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -651,6 +663,10 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Rusks.png</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -674,6 +690,10 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Spinach.png</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -697,6 +717,10 @@
       <c r="H9">
         <v>0</v>
       </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>lemon.png</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -720,6 +744,10 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>eggplant.png</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -743,6 +771,10 @@
       <c r="H11">
         <v>0</v>
       </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>melon.png</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -766,6 +798,10 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>soup.png</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
@@ -789,6 +825,10 @@
       <c r="H13">
         <v>4</v>
       </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>strawberry.png</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -812,6 +852,10 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>sweetcorn.png</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -835,6 +879,10 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>cookies.png</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -858,8 +906,12 @@
       <c r="H16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>Maggi.png</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -881,8 +933,12 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>noodles.png</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -904,8 +960,12 @@
       <c r="H18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>indiagaterice.png</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -927,8 +987,12 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>mangoes.png</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -950,8 +1014,12 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>onion.png</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -973,8 +1041,12 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>Rusks.png</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -996,8 +1068,12 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>Spinach.png</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -1019,8 +1095,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>lemon.png</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>16</v>
       </c>
@@ -1042,8 +1122,12 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>eggplant.png</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -1065,8 +1149,12 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>melon.png</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1088,8 +1176,12 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>soup.png</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -1111,8 +1203,12 @@
       <c r="H27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>strawberry.png</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>20</v>
       </c>
@@ -1134,8 +1230,12 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>sweetcorn.png</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -1157,8 +1257,12 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>cookies.png</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -1180,8 +1284,12 @@
       <c r="H30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>Maggi.png</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>8</v>
       </c>
@@ -1203,8 +1311,12 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>noodles.png</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1226,8 +1338,12 @@
       <c r="H32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>indiagaterice.png</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>10</v>
       </c>
@@ -1249,8 +1365,12 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>mangoes.png</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -1272,8 +1392,12 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>onion.png</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>13</v>
       </c>
@@ -1295,8 +1419,12 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>Rusks.png</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>14</v>
       </c>
@@ -1318,8 +1446,12 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>Spinach.png</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>15</v>
       </c>
@@ -1341,8 +1473,12 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>lemon.png</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>16</v>
       </c>
@@ -1364,8 +1500,12 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>eggplant.png</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>17</v>
       </c>
@@ -1387,8 +1527,12 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>melon.png</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>18</v>
       </c>
@@ -1410,8 +1554,12 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>soup.png</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -1433,8 +1581,12 @@
       <c r="H41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>strawberry.png</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>20</v>
       </c>
@@ -1456,8 +1608,12 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>sweetcorn.png</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>21</v>
       </c>
@@ -1479,8 +1635,12 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>cookies.png</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>11</v>
       </c>
@@ -1502,8 +1662,12 @@
       <c r="H44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>Maggi.png</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -1525,8 +1689,12 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>noodles.png</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>9</v>
       </c>
@@ -1548,8 +1716,12 @@
       <c r="H46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>indiagaterice.png</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>10</v>
       </c>
@@ -1571,8 +1743,12 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>mangoes.png</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>12</v>
       </c>
@@ -1594,8 +1770,12 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>onion.png</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>13</v>
       </c>
@@ -1617,8 +1797,12 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>Rusks.png</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>14</v>
       </c>
@@ -1640,8 +1824,12 @@
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>Spinach.png</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>15</v>
       </c>
@@ -1663,8 +1851,12 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>lemon.png</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>16</v>
       </c>
@@ -1686,8 +1878,12 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>eggplant.png</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>17</v>
       </c>
@@ -1709,8 +1905,12 @@
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>melon.png</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>18</v>
       </c>
@@ -1732,8 +1932,12 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>soup.png</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>19</v>
       </c>
@@ -1755,8 +1959,12 @@
       <c r="H55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>strawberry.png</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>20</v>
       </c>
@@ -1778,8 +1986,12 @@
       <c r="H56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="str">
+        <f t="shared" si="0"/>
+        <v>sweetcorn.png</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>21</v>
       </c>
@@ -1800,6 +2012,10 @@
       </c>
       <c r="H57">
         <v>0</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>cookies.png</v>
       </c>
     </row>
   </sheetData>

</xml_diff>